<commit_message>
Latest version of code and results
</commit_message>
<xml_diff>
--- a/Matlab-code/tests for Jin/Matlab Code_For_Loren/Physiology_Output/Physiology_Variable_Master_Sheet.xlsx
+++ b/Matlab-code/tests for Jin/Matlab Code_For_Loren/Physiology_Output/Physiology_Variable_Master_Sheet.xlsx
@@ -527,10 +527,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.77166665431477321</v>
+        <v>0.78329501310442828</v>
       </c>
       <c r="D2">
-        <v>2.0991495917622012</v>
+        <v>1.8466738095600985</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -539,34 +539,34 @@
         <v>30.398000000000007</v>
       </c>
       <c r="G2">
-        <v>29.997117099517379</v>
+        <v>0.10000405272976591</v>
       </c>
       <c r="H2">
-        <v>17.733319547182017</v>
+        <v>24.913461023337664</v>
       </c>
       <c r="I2">
-        <v>9.9999988755088793</v>
+        <v>15.621224892810893</v>
       </c>
       <c r="J2">
-        <v>72.288410765383233</v>
+        <v>104.64310411888128</v>
       </c>
       <c r="K2">
-        <v>36.77486816313737</v>
+        <v>34.752449315596806</v>
       </c>
       <c r="L2">
-        <v>21.158159392307638</v>
+        <v>7.0536834606921867E-2</v>
       </c>
       <c r="M2">
-        <v>11.101277426856232</v>
+        <v>15.596134821085466</v>
       </c>
       <c r="N2">
-        <v>7.1659462478209486</v>
+        <v>11.194087049465692</v>
       </c>
       <c r="O2">
-        <v>52.76096488333625</v>
+        <v>76.375605484239955</v>
       </c>
       <c r="P2">
-        <v>28.250555270120444</v>
+        <v>26.696927526893106</v>
       </c>
       <c r="Q2">
         <v>1.4177564571341339</v>
@@ -592,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.98756025550592552</v>
+        <v>0.98990221819709978</v>
       </c>
       <c r="D3">
-        <v>0.69426725728473737</v>
+        <v>0.56283192302931706</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -604,34 +604,34 @@
         <v>30.495000000000005</v>
       </c>
       <c r="G3">
-        <v>0.15961959363901271</v>
+        <v>0.1224401060204636</v>
       </c>
       <c r="H3">
-        <v>30.941767930988235</v>
+        <v>37.136149086996575</v>
       </c>
       <c r="I3">
-        <v>9.9979535573630844</v>
+        <v>12.501858021838444</v>
       </c>
       <c r="J3">
-        <v>101.31364751079798</v>
+        <v>112.94276154022478</v>
       </c>
       <c r="K3">
-        <v>55.902276078468383</v>
+        <v>62.767671748572312</v>
       </c>
       <c r="L3">
-        <v>0.11192725787757905</v>
+        <v>8.5856535583618054E-2</v>
       </c>
       <c r="M3">
-        <v>19.21040978477459</v>
+        <v>23.056233999971766</v>
       </c>
       <c r="N3">
-        <v>7.1225334004541576</v>
+        <v>8.906312758644706</v>
       </c>
       <c r="O3">
-        <v>73.53577461632112</v>
+        <v>81.976452938205483</v>
       </c>
       <c r="P3">
-        <v>42.815776948974758</v>
+        <v>48.074010965511434</v>
       </c>
       <c r="Q3">
         <v>1.4261011720093899</v>
@@ -657,10 +657,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.96353459060303115</v>
+        <v>0.96353449056561224</v>
       </c>
       <c r="D4">
-        <v>0.83754855046985743</v>
+        <v>0.83754989478856323</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -669,34 +669,34 @@
         <v>29.891818181818181</v>
       </c>
       <c r="G4">
-        <v>0.10000001575606052</v>
+        <v>0.10000031088873702</v>
       </c>
       <c r="H4">
-        <v>22.319555313525438</v>
+        <v>22.294682946419176</v>
       </c>
       <c r="I4">
-        <v>9.8130605550506083</v>
+        <v>9.7950315256722238</v>
       </c>
       <c r="J4">
-        <v>86.385141343898184</v>
+        <v>109.05095718685831</v>
       </c>
       <c r="K4">
-        <v>42.922332854750209</v>
+        <v>35.557215284075696</v>
       </c>
       <c r="L4">
-        <v>7.2756007980306334E-2</v>
+        <v>7.2756222707026169E-2</v>
       </c>
       <c r="M4">
-        <v>14.589723738652678</v>
+        <v>14.573465306989981</v>
       </c>
       <c r="N4">
-        <v>7.2512441602522761</v>
+        <v>7.2379218238352507</v>
       </c>
       <c r="O4">
-        <v>64.908537461630345</v>
+        <v>81.93930147791346</v>
       </c>
       <c r="P4">
-        <v>33.536650753055596</v>
+        <v>27.782038659655161</v>
       </c>
       <c r="Q4">
         <v>1.3744571552514071</v>
@@ -722,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.93874499170605064</v>
+        <v>0.9387437250173003</v>
       </c>
       <c r="D5">
-        <v>0.73984885056045335</v>
+        <v>0.72308013428846418</v>
       </c>
       <c r="E5">
         <v>11</v>
@@ -734,34 +734,34 @@
         <v>30.108181818181819</v>
       </c>
       <c r="G5">
-        <v>0.10000811753601128</v>
+        <v>0.10001263668525223</v>
       </c>
       <c r="H5">
-        <v>15.819689924926175</v>
+        <v>16.741674786246577</v>
       </c>
       <c r="I5">
-        <v>8.5699165700973374</v>
+        <v>9.2406868972764755</v>
       </c>
       <c r="J5">
-        <v>92.741015435937058</v>
+        <v>71.585968678588344</v>
       </c>
       <c r="K5">
-        <v>26.48030712746062</v>
+        <v>23.550555029466061</v>
       </c>
       <c r="L5">
-        <v>7.1798148441771278E-2</v>
+        <v>7.1801392843886092E-2</v>
       </c>
       <c r="M5">
-        <v>10.151379132070426</v>
+        <v>10.743010063252312</v>
       </c>
       <c r="N5">
-        <v>6.2499923197842042</v>
+        <v>6.7391813753506025</v>
       </c>
       <c r="O5">
-        <v>68.823331020125948</v>
+        <v>53.124119847125691</v>
       </c>
       <c r="P5">
-        <v>20.535197750263844</v>
+        <v>18.263206024413417</v>
       </c>
       <c r="Q5">
         <v>1.3929066376567978</v>
@@ -787,10 +787,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.97692808371592343</v>
+        <v>0.9769215571354265</v>
       </c>
       <c r="D6">
-        <v>1.9166775851563811</v>
+        <v>1.1171792241720118</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -799,34 +799,34 @@
         <v>30.009999999999998</v>
       </c>
       <c r="G6">
-        <v>0.10007508644159567</v>
+        <v>0.10019816388634087</v>
       </c>
       <c r="H6">
-        <v>27.420590315781855</v>
+        <v>33.972219610744872</v>
       </c>
       <c r="I6">
-        <v>9.9999560868877406</v>
+        <v>14.876994251487275</v>
       </c>
       <c r="J6">
-        <v>116.75046274203504</v>
+        <v>133.9527813567716</v>
       </c>
       <c r="K6">
-        <v>65.630490946437519</v>
+        <v>62.148068854647647</v>
       </c>
       <c r="L6">
-        <v>7.228130335214876E-2</v>
+        <v>7.2370198585075957E-2</v>
       </c>
       <c r="M6">
-        <v>17.743869909608968</v>
+        <v>21.983430639959064</v>
       </c>
       <c r="N6">
-        <v>7.3364991159178512</v>
+        <v>10.91455344655621</v>
       </c>
       <c r="O6">
-        <v>87.130746222618285</v>
+        <v>99.968818316370971</v>
       </c>
       <c r="P6">
-        <v>51.067004595395119</v>
+        <v>48.357336232413111</v>
       </c>
       <c r="Q6">
         <v>1.3845224394202995</v>
@@ -852,10 +852,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.99158102928822611</v>
+        <v>0.99158087810887074</v>
       </c>
       <c r="D7">
-        <v>0.45666383159605922</v>
+        <v>0.45670297870571192</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -864,34 +864,34 @@
         <v>30.024000000000001</v>
       </c>
       <c r="G7">
-        <v>0.10733492924419008</v>
+        <v>0.10747930643896778</v>
       </c>
       <c r="H7">
-        <v>25.304141247459519</v>
+        <v>25.329025461355727</v>
       </c>
       <c r="I7">
-        <v>9.1028261600535814</v>
+        <v>9.1195880696007201</v>
       </c>
       <c r="J7">
-        <v>108.044495055</v>
+        <v>109.76788687285288</v>
       </c>
       <c r="K7">
-        <v>45.963085280870665</v>
+        <v>52.75875054074892</v>
       </c>
       <c r="L7">
-        <v>7.7458057383248832E-2</v>
+        <v>7.7562246924497619E-2</v>
       </c>
       <c r="M7">
-        <v>16.354728163298041</v>
+        <v>16.370811481433595</v>
       </c>
       <c r="N7">
-        <v>6.6726433040451303</v>
+        <v>6.6849302841034275</v>
       </c>
       <c r="O7">
-        <v>80.568664258073909</v>
+        <v>81.853795691073046</v>
       </c>
       <c r="P7">
-        <v>35.746519642032808</v>
+        <v>41.031660537350803</v>
       </c>
       <c r="Q7">
         <v>1.3857167720217374</v>
@@ -917,10 +917,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.9633100932813371</v>
+        <v>0.96332099721190789</v>
       </c>
       <c r="D8">
-        <v>0.54807382062989785</v>
+        <v>0.54798800107340739</v>
       </c>
       <c r="E8">
         <v>14</v>
@@ -929,34 +929,34 @@
         <v>30.6</v>
       </c>
       <c r="G8">
-        <v>0.1000917461330417</v>
+        <v>0.10000883164966745</v>
       </c>
       <c r="H8">
-        <v>16.268574807562846</v>
+        <v>16.288500460874836</v>
       </c>
       <c r="I8">
-        <v>9.5864722877075508</v>
+        <v>9.6071903359183342</v>
       </c>
       <c r="J8">
-        <v>68.540918748754621</v>
+        <v>81.456096172891918</v>
       </c>
       <c r="K8">
-        <v>26.71390245601717</v>
+        <v>30.840152337899877</v>
       </c>
       <c r="L8">
-        <v>6.9743252110632648E-2</v>
+        <v>6.9685477859098399E-2</v>
       </c>
       <c r="M8">
-        <v>10.010505028607072</v>
+        <v>10.022765835410212</v>
       </c>
       <c r="N8">
-        <v>6.7861506071964453</v>
+        <v>6.8008166690413026</v>
       </c>
       <c r="O8">
-        <v>49.450422872088794</v>
+        <v>58.768374786809055</v>
       </c>
       <c r="P8">
-        <v>20.395946508881998</v>
+        <v>23.546320064813138</v>
       </c>
       <c r="Q8">
         <v>1.4351459546834395</v>
@@ -982,10 +982,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.98133402306135797</v>
+        <v>0.98237650834681167</v>
       </c>
       <c r="D9">
-        <v>0.83819932604921821</v>
+        <v>0.62011373959013427</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -994,34 +994,34 @@
         <v>31.152222222222221</v>
       </c>
       <c r="G9">
-        <v>0.2926130431196981</v>
+        <v>0.2235730917971317</v>
       </c>
       <c r="H9">
-        <v>25.519364976845676</v>
+        <v>28.617916164324047</v>
       </c>
       <c r="I9">
-        <v>9.9995698189324269</v>
+        <v>11.827221251124925</v>
       </c>
       <c r="J9">
-        <v>94.900122353141526</v>
+        <v>106.81211596992512</v>
       </c>
       <c r="K9">
-        <v>38.534847355918657</v>
+        <v>27.914289772664617</v>
       </c>
       <c r="L9">
-        <v>0.19733825592768747</v>
+        <v>0.15077770811999974</v>
       </c>
       <c r="M9">
-        <v>14.982632174265586</v>
+        <v>16.801817438367742</v>
       </c>
       <c r="N9">
-        <v>6.8464993480913892</v>
+        <v>8.0978546129301865</v>
       </c>
       <c r="O9">
-        <v>66.341688777002474</v>
+        <v>74.668988612271193</v>
       </c>
       <c r="P9">
-        <v>28.986641664422173</v>
+        <v>20.997657198006159</v>
       </c>
       <c r="Q9">
         <v>1.482799377870873</v>
@@ -1047,10 +1047,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.96798372855984616</v>
+        <v>0.96798126390294659</v>
       </c>
       <c r="D10">
-        <v>0.58240876362276128</v>
+        <v>0.58434587666726401</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -1059,34 +1059,34 @@
         <v>30.323</v>
       </c>
       <c r="G10">
-        <v>0.10000703495565173</v>
+        <v>0.10001559407935941</v>
       </c>
       <c r="H10">
-        <v>18.18879158932166</v>
+        <v>18.085118965196308</v>
       </c>
       <c r="I10">
-        <v>8.7587131034605434</v>
+        <v>8.7066131941273479</v>
       </c>
       <c r="J10">
-        <v>81.238521794050214</v>
+        <v>68.751400329459344</v>
       </c>
       <c r="K10">
-        <v>28.501082818390984</v>
+        <v>24.226209772259221</v>
       </c>
       <c r="L10">
-        <v>7.0860993684911638E-2</v>
+        <v>7.0867058338375935E-2</v>
       </c>
       <c r="M10">
-        <v>11.45948766021051</v>
+        <v>11.394170778050862</v>
       </c>
       <c r="N10">
-        <v>6.3050252440102437</v>
+        <v>6.2675207339667924</v>
       </c>
       <c r="O10">
-        <v>59.548811821789279</v>
+        <v>50.395601868316106</v>
       </c>
       <c r="P10">
-        <v>21.94664592913206</v>
+        <v>18.65487186801095</v>
       </c>
       <c r="Q10">
         <v>1.4113129065101739</v>
@@ -1112,10 +1112,10 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.7509752976950369</v>
+        <v>0.75097529748476766</v>
       </c>
       <c r="D11">
-        <v>0.40883560643036732</v>
+        <v>0.40883560796923629</v>
       </c>
       <c r="E11">
         <v>14</v>
@@ -1124,34 +1124,34 @@
         <v>30.659285714285708</v>
       </c>
       <c r="G11">
-        <v>29.96832796740944</v>
+        <v>29.85426286542269</v>
       </c>
       <c r="H11">
-        <v>6.3410987139224222</v>
+        <v>6.3415887275175846</v>
       </c>
       <c r="I11">
-        <v>4.7364651675786202</v>
+        <v>4.736850224554324</v>
       </c>
       <c r="J11">
-        <v>25.558598337143646</v>
+        <v>52.034610543388993</v>
       </c>
       <c r="K11">
-        <v>6.6581914422418684</v>
+        <v>7.046652307766065</v>
       </c>
       <c r="L11">
-        <v>20.807620949300215</v>
+        <v>20.728423224012886</v>
       </c>
       <c r="M11">
-        <v>3.8822061576505424</v>
+        <v>3.8825061583100964</v>
       </c>
       <c r="N11">
-        <v>3.34089037743869</v>
+        <v>3.3411619793822029</v>
       </c>
       <c r="O11">
-        <v>18.377392365120848</v>
+        <v>37.414432587737224</v>
       </c>
       <c r="P11">
-        <v>5.0746912694291195</v>
+        <v>5.3707655081906838</v>
       </c>
       <c r="Q11">
         <v>1.440257299978223</v>
@@ -1177,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.99683015617962312</v>
+        <v>0.99683168511846221</v>
       </c>
       <c r="D12">
-        <v>0.20880222400637805</v>
+        <v>0.20871156917643785</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -1189,34 +1189,34 @@
         <v>30.63111111111111</v>
       </c>
       <c r="G12">
-        <v>0.16113101599448873</v>
+        <v>0.16135302220977976</v>
       </c>
       <c r="H12">
-        <v>17.946722623269117</v>
+        <v>17.931653379531369</v>
       </c>
       <c r="I12">
-        <v>7.3954537131502924</v>
+        <v>7.3795891155854596</v>
       </c>
       <c r="J12">
-        <v>98.903972521030383</v>
+        <v>68.480224050215668</v>
       </c>
       <c r="K12">
-        <v>32.589282210045383</v>
+        <v>24.151418513943053</v>
       </c>
       <c r="L12">
-        <v>0.11206558169582129</v>
+        <v>0.11221998558574356</v>
       </c>
       <c r="M12">
-        <v>11.013897420091398</v>
+        <v>11.004649430460649</v>
       </c>
       <c r="N12">
-        <v>5.2253148944400172</v>
+        <v>5.2141056405976993</v>
       </c>
       <c r="O12">
-        <v>71.229623651118899</v>
+        <v>49.318752951040167</v>
       </c>
       <c r="P12">
-        <v>24.859039641151536</v>
+        <v>18.422653998899335</v>
       </c>
       <c r="Q12">
         <v>1.4378278643289906</v>
@@ -1242,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.95958692438487403</v>
+        <v>0.95943866745095074</v>
       </c>
       <c r="D13">
-        <v>1.0846484069140934</v>
+        <v>1.0873018463492452</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -1254,34 +1254,34 @@
         <v>30.440909090909091</v>
       </c>
       <c r="G13">
-        <v>0.10001927035294039</v>
+        <v>0.10006922382184548</v>
       </c>
       <c r="H13">
-        <v>27.972944956887854</v>
+        <v>27.423475529793642</v>
       </c>
       <c r="I13">
-        <v>9.8687232476295002</v>
+        <v>9.5928219279264368</v>
       </c>
       <c r="J13">
-        <v>97.910729698688982</v>
+        <v>97.066218998087578</v>
       </c>
       <c r="K13">
-        <v>53.317564646467694</v>
+        <v>48.230761019648163</v>
       </c>
       <c r="L13">
-        <v>7.0364433156929099E-2</v>
+        <v>7.0399575860043459E-2</v>
       </c>
       <c r="M13">
-        <v>17.447456357034959</v>
+        <v>17.104737924509298</v>
       </c>
       <c r="N13">
-        <v>7.0535255890327493</v>
+        <v>6.8563291564505588</v>
       </c>
       <c r="O13">
-        <v>71.286383644823061</v>
+        <v>70.671516265318317</v>
       </c>
       <c r="P13">
-        <v>40.90401780173169</v>
+        <v>37.001538243916322</v>
       </c>
       <c r="Q13">
         <v>1.4214464021883626</v>
@@ -1307,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.97326544895070555</v>
+        <v>0.97326813102549958</v>
       </c>
       <c r="D14">
-        <v>0.39612059290263074</v>
+        <v>0.39611002820300767</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1319,34 +1319,34 @@
         <v>30.852999999999998</v>
       </c>
       <c r="G14">
-        <v>0.1000285346558602</v>
+        <v>0.10001208672522731</v>
       </c>
       <c r="H14">
-        <v>13.353680174233412</v>
+        <v>13.362410821891572</v>
       </c>
       <c r="I14">
-        <v>5.8785547192974086</v>
+        <v>5.883613364416461</v>
       </c>
       <c r="J14">
-        <v>78.533383146638627</v>
+        <v>67.517462252747904</v>
       </c>
       <c r="K14">
-        <v>22.209777369789141</v>
+        <v>28.363171934830547</v>
       </c>
       <c r="L14">
-        <v>6.8655025391507724E-2</v>
+        <v>6.8643736281863918E-2</v>
       </c>
       <c r="M14">
-        <v>8.0418767588864704</v>
+        <v>8.0471345448732627</v>
       </c>
       <c r="N14">
-        <v>4.0982259217705863</v>
+        <v>4.1017525489001905</v>
       </c>
       <c r="O14">
-        <v>55.845916458837181</v>
+        <v>48.012379008799137</v>
       </c>
       <c r="P14">
-        <v>16.835833369944609</v>
+        <v>21.500334226107103</v>
       </c>
       <c r="Q14">
         <v>1.4569732380906413</v>
@@ -1372,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.82714348277108141</v>
+        <v>0.82714350169032713</v>
       </c>
       <c r="D15">
-        <v>1.0560440103867934</v>
+        <v>0.96125685126048033</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -1384,34 +1384,34 @@
         <v>31.269999999999996</v>
       </c>
       <c r="G15">
-        <v>29.930659896123085</v>
+        <v>29.987713859243719</v>
       </c>
       <c r="H15">
-        <v>15.493230799955473</v>
+        <v>19.562202927333093</v>
       </c>
       <c r="I15">
-        <v>9.9999986014305939</v>
+        <v>13.15852159410127</v>
       </c>
       <c r="J15">
-        <v>75.399757622746549</v>
+        <v>83.044575098429405</v>
       </c>
       <c r="K15">
-        <v>21.693121680926954</v>
+        <v>11.958649945618919</v>
       </c>
       <c r="L15">
-        <v>20.047985969970462</v>
+        <v>20.086201534082424</v>
       </c>
       <c r="M15">
-        <v>9.0057818214812144</v>
+        <v>11.37096153706103</v>
       </c>
       <c r="N15">
-        <v>6.7983927401410345</v>
+        <v>8.9456810187482905</v>
       </c>
       <c r="O15">
-        <v>52.356924467638677</v>
+        <v>57.665418072430604</v>
       </c>
       <c r="P15">
-        <v>16.272473611805381</v>
+        <v>8.9704385811837923</v>
       </c>
       <c r="Q15">
         <v>1.4929509598099138</v>

</xml_diff>